<commit_message>
updated w new stats 2020-03-24
</commit_message>
<xml_diff>
--- a/region_names.xlsx
+++ b/region_names.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mortenjc/proj/covid2019/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D83DBE2-C8D8-0940-95B3-23111B5AF169}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99D92E53-8E68-7942-BC5A-7EF0D04A4465}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10020" yWindow="460" windowWidth="16840" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="196">
   <si>
     <t>Countries.and.territories</t>
   </si>
@@ -602,6 +602,12 @@
   </si>
   <si>
     <t>Syria</t>
+  </si>
+  <si>
+    <t>Belize</t>
+  </si>
+  <si>
+    <t>United_States_Virgin_Islands</t>
   </si>
 </sst>
 </file>
@@ -953,10 +959,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B185"/>
+  <dimension ref="A1:B187"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" topLeftCell="A152" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B181" sqref="B181"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1110,7 +1116,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>17</v>
+        <v>194</v>
       </c>
       <c r="B19" t="s">
         <v>157</v>
@@ -1118,7 +1124,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>187</v>
+        <v>17</v>
       </c>
       <c r="B20" t="s">
         <v>157</v>
@@ -1126,87 +1132,87 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>18</v>
+        <v>187</v>
       </c>
       <c r="B21" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B22" t="s">
-        <v>158</v>
+        <v>165</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B23" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B24" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B25" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B26" t="s">
-        <v>157</v>
+        <v>165</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B27" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B28" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B29" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B30" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B31" t="s">
         <v>162</v>
@@ -1214,23 +1220,23 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>186</v>
+        <v>28</v>
       </c>
       <c r="B32" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>29</v>
+        <v>186</v>
       </c>
       <c r="B33" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>185</v>
+        <v>29</v>
       </c>
       <c r="B34" t="s">
         <v>157</v>
@@ -1238,15 +1244,15 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>30</v>
+        <v>185</v>
       </c>
       <c r="B35" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>184</v>
+        <v>30</v>
       </c>
       <c r="B36" t="s">
         <v>161</v>
@@ -1254,79 +1260,79 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>31</v>
+        <v>184</v>
       </c>
       <c r="B37" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B38" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B39" t="s">
-        <v>158</v>
+        <v>165</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B40" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B41" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B42" t="s">
-        <v>157</v>
+        <v>162</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B43" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B44" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B45" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B46" t="s">
         <v>159</v>
@@ -1334,31 +1340,31 @@
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B47" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B48" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B49" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>190</v>
+        <v>43</v>
       </c>
       <c r="B50" t="s">
         <v>157</v>
@@ -1366,7 +1372,7 @@
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>44</v>
+        <v>190</v>
       </c>
       <c r="B51" t="s">
         <v>157</v>
@@ -1374,31 +1380,31 @@
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B52" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B53" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B54" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B55" t="s">
         <v>157</v>
@@ -1406,63 +1412,63 @@
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>183</v>
+        <v>48</v>
       </c>
       <c r="B56" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>49</v>
+        <v>183</v>
       </c>
       <c r="B57" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B58" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B59" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>182</v>
+        <v>51</v>
       </c>
       <c r="B60" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B61" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>52</v>
+        <v>181</v>
       </c>
       <c r="B62" t="s">
-        <v>159</v>
+        <v>165</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B63" t="s">
         <v>159</v>
@@ -1470,15 +1476,15 @@
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B64" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B65" t="s">
         <v>157</v>
@@ -1486,47 +1492,47 @@
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B66" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B67" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B68" t="s">
-        <v>159</v>
+        <v>165</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B69" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>180</v>
+        <v>59</v>
       </c>
       <c r="B70" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>60</v>
+        <v>180</v>
       </c>
       <c r="B71" t="s">
         <v>159</v>
@@ -1534,31 +1540,31 @@
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>191</v>
+        <v>60</v>
       </c>
       <c r="B72" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="B73" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>61</v>
+        <v>189</v>
       </c>
       <c r="B74" t="s">
-        <v>157</v>
+        <v>162</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B75" t="s">
         <v>157</v>
@@ -1566,39 +1572,39 @@
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>179</v>
+        <v>62</v>
       </c>
       <c r="B76" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>63</v>
+        <v>179</v>
       </c>
       <c r="B77" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B78" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>178</v>
+        <v>64</v>
       </c>
       <c r="B79" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>65</v>
+        <v>178</v>
       </c>
       <c r="B80" t="s">
         <v>157</v>
@@ -1606,7 +1612,7 @@
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B81" t="s">
         <v>157</v>
@@ -1614,15 +1620,15 @@
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B82" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B83" t="s">
         <v>159</v>
@@ -1630,15 +1636,15 @@
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B84" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B85" t="s">
         <v>165</v>
@@ -1646,7 +1652,7 @@
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B86" t="s">
         <v>165</v>
@@ -1654,23 +1660,23 @@
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B87" t="s">
-        <v>157</v>
+        <v>165</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B88" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>177</v>
+        <v>73</v>
       </c>
       <c r="B89" t="s">
         <v>159</v>
@@ -1678,55 +1684,55 @@
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>74</v>
+        <v>177</v>
       </c>
       <c r="B90" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B91" t="s">
-        <v>159</v>
+        <v>165</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B92" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B93" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>176</v>
+        <v>77</v>
       </c>
       <c r="B94" t="s">
-        <v>159</v>
+        <v>165</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>78</v>
+        <v>176</v>
       </c>
       <c r="B95" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B96" t="s">
         <v>165</v>
@@ -1734,31 +1740,31 @@
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B97" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B98" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B99" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B100" t="s">
         <v>165</v>
@@ -1766,39 +1772,39 @@
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B101" t="s">
-        <v>159</v>
+        <v>165</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B102" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B103" t="s">
-        <v>157</v>
+        <v>165</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B104" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B105" t="s">
         <v>159</v>
@@ -1806,7 +1812,7 @@
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B106" t="s">
         <v>159</v>
@@ -1814,23 +1820,23 @@
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>175</v>
+        <v>89</v>
       </c>
       <c r="B107" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>90</v>
+        <v>175</v>
       </c>
       <c r="B108" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B109" t="s">
         <v>165</v>
@@ -1838,23 +1844,23 @@
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B110" t="s">
-        <v>159</v>
+        <v>165</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B111" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>174</v>
+        <v>93</v>
       </c>
       <c r="B112" t="s">
         <v>157</v>
@@ -1862,47 +1868,47 @@
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>94</v>
+        <v>174</v>
       </c>
       <c r="B113" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B114" t="s">
-        <v>157</v>
+        <v>162</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B115" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B116" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B117" t="s">
-        <v>157</v>
+        <v>165</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>173</v>
+        <v>98</v>
       </c>
       <c r="B118" t="s">
         <v>157</v>
@@ -1910,15 +1916,15 @@
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>99</v>
+        <v>173</v>
       </c>
       <c r="B119" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>192</v>
+        <v>99</v>
       </c>
       <c r="B120" t="s">
         <v>161</v>
@@ -1926,47 +1932,47 @@
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>100</v>
+        <v>192</v>
       </c>
       <c r="B121" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B122" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B123" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B124" t="s">
-        <v>159</v>
+        <v>165</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>172</v>
+        <v>103</v>
       </c>
       <c r="B125" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B126" t="s">
         <v>157</v>
@@ -1974,31 +1980,31 @@
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>104</v>
+        <v>171</v>
       </c>
       <c r="B127" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B128" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>170</v>
+        <v>105</v>
       </c>
       <c r="B129" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>106</v>
+        <v>170</v>
       </c>
       <c r="B130" t="s">
         <v>161</v>
@@ -2006,15 +2012,15 @@
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B131" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B132" t="s">
         <v>159</v>
@@ -2022,23 +2028,23 @@
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B133" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B134" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B135" t="s">
         <v>165</v>
@@ -2046,31 +2052,31 @@
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B136" t="s">
-        <v>158</v>
+        <v>165</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>169</v>
+        <v>112</v>
       </c>
       <c r="B137" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>113</v>
+        <v>169</v>
       </c>
       <c r="B138" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B139" t="s">
         <v>158</v>
@@ -2078,23 +2084,23 @@
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B140" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B141" t="s">
-        <v>159</v>
+        <v>165</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B142" t="s">
         <v>159</v>
@@ -2102,23 +2108,23 @@
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B143" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B144" t="s">
-        <v>159</v>
+        <v>165</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B145" t="s">
         <v>159</v>
@@ -2126,23 +2132,23 @@
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B146" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B147" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B148" t="s">
         <v>157</v>
@@ -2150,63 +2156,63 @@
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B149" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B150" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B151" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B152" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B153" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B154" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B155" t="s">
-        <v>159</v>
+        <v>165</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B156" t="s">
         <v>159</v>
@@ -2214,15 +2220,15 @@
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B157" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B158" t="s">
         <v>161</v>
@@ -2230,55 +2236,55 @@
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B159" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B160" t="s">
-        <v>159</v>
+        <v>165</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B161" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B162" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B163" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B164" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B165" t="s">
         <v>159</v>
@@ -2286,15 +2292,15 @@
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
-        <v>193</v>
+        <v>140</v>
       </c>
       <c r="B166" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
-        <v>141</v>
+        <v>193</v>
       </c>
       <c r="B167" t="s">
         <v>165</v>
@@ -2302,7 +2308,7 @@
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B168" t="s">
         <v>165</v>
@@ -2310,15 +2316,15 @@
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
-        <v>168</v>
+        <v>142</v>
       </c>
       <c r="B169" t="s">
-        <v>157</v>
+        <v>165</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
-        <v>143</v>
+        <v>168</v>
       </c>
       <c r="B170" t="s">
         <v>157</v>
@@ -2326,7 +2332,7 @@
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B171" t="s">
         <v>157</v>
@@ -2334,87 +2340,87 @@
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B172" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B173" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
-        <v>167</v>
+        <v>146</v>
       </c>
       <c r="B174" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
-        <v>147</v>
+        <v>167</v>
       </c>
       <c r="B175" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B176" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B177" t="s">
-        <v>157</v>
+        <v>165</v>
       </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B178" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B179" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B180" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
-        <v>153</v>
+        <v>195</v>
       </c>
       <c r="B181" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B182" t="s">
         <v>158</v>
@@ -2422,7 +2428,7 @@
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B183" t="s">
         <v>165</v>
@@ -2430,17 +2436,33 @@
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B184" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
+        <v>155</v>
+      </c>
+      <c r="B185" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="186" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A186" t="s">
+        <v>156</v>
+      </c>
+      <c r="B186" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="187" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A187" t="s">
         <v>166</v>
       </c>
-      <c r="B185" t="s">
+      <c r="B187" t="s">
         <v>161</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated countries and excel schema
</commit_message>
<xml_diff>
--- a/region_names.xlsx
+++ b/region_names.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mortenjc/proj/covid2019/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99D92E53-8E68-7942-BC5A-7EF0D04A4465}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81684CD5-125C-2D47-A6BC-56DB17F297B6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10020" yWindow="460" windowWidth="16840" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6880" yWindow="460" windowWidth="16840" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="countries" sheetId="1" r:id="rId1"/>
@@ -20,10 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="196">
-  <si>
-    <t>Countries.and.territories</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="204">
   <si>
     <t>Afghanistan</t>
   </si>
@@ -103,9 +100,6 @@
     <t>Cameroon</t>
   </si>
   <si>
-    <t>CANADA</t>
-  </si>
-  <si>
     <t>Canada</t>
   </si>
   <si>
@@ -493,9 +487,6 @@
     <t>Zambia</t>
   </si>
   <si>
-    <t>na</t>
-  </si>
-  <si>
     <t>south america</t>
   </si>
   <si>
@@ -538,9 +529,6 @@
     <t>New_Caledonia</t>
   </si>
   <si>
-    <t>Netherlands_Antilles</t>
-  </si>
-  <si>
     <t>Montserrat</t>
   </si>
   <si>
@@ -608,6 +596,42 @@
   </si>
   <si>
     <t>United_States_Virgin_Islands</t>
+  </si>
+  <si>
+    <t>Curaçao</t>
+  </si>
+  <si>
+    <t>Laos</t>
+  </si>
+  <si>
+    <t>Libya</t>
+  </si>
+  <si>
+    <t>Mali</t>
+  </si>
+  <si>
+    <t>Saint_Kitts_and_Nevis</t>
+  </si>
+  <si>
+    <t>Sint_Maarten</t>
+  </si>
+  <si>
+    <t>Turks_and_Caicos_islands</t>
+  </si>
+  <si>
+    <t>Aruba</t>
+  </si>
+  <si>
+    <t>Anguilla</t>
+  </si>
+  <si>
+    <t>British_Virgin_Islands</t>
+  </si>
+  <si>
+    <t>Guinea_Bissau</t>
+  </si>
+  <si>
+    <t>countriesAndTerritories</t>
   </si>
 </sst>
 </file>
@@ -959,11 +983,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B187"/>
+  <dimension ref="A1:B196"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A152" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B181" sqref="B181"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -972,63 +994,63 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>203</v>
       </c>
       <c r="B1" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>184</v>
       </c>
       <c r="B3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>188</v>
+        <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B8" t="s">
         <v>158</v>
@@ -1036,23 +1058,23 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>200</v>
       </c>
       <c r="B9" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B10" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>9</v>
+        <v>199</v>
       </c>
       <c r="B11" t="s">
         <v>159</v>
@@ -1060,55 +1082,55 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B12" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B13" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B14" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B15" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B16" t="s">
-        <v>157</v>
+        <v>162</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B17" t="s">
-        <v>157</v>
+        <v>162</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B18" t="s">
         <v>159</v>
@@ -1116,111 +1138,111 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>194</v>
+        <v>14</v>
       </c>
       <c r="B19" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B20" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="B21" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B22" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>19</v>
+        <v>183</v>
       </c>
       <c r="B23" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B24" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B25" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B26" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B27" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>24</v>
+        <v>201</v>
       </c>
       <c r="B28" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B29" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B30" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B31" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B32" t="s">
         <v>162</v>
@@ -1228,47 +1250,47 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>186</v>
+        <v>25</v>
       </c>
       <c r="B33" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B34" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="B35" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B36" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="B37" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B38" t="s">
         <v>158</v>
@@ -1276,47 +1298,47 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>32</v>
+        <v>180</v>
       </c>
       <c r="B39" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B40" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B41" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B42" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B43" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B44" t="s">
         <v>159</v>
@@ -1324,23 +1346,23 @@
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B45" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B46" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B47" t="s">
         <v>159</v>
@@ -1348,47 +1370,47 @@
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>41</v>
+        <v>192</v>
       </c>
       <c r="B48" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B49" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B50" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>190</v>
+        <v>39</v>
       </c>
       <c r="B51" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B52" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B53" t="s">
         <v>158</v>
@@ -1396,39 +1418,39 @@
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>46</v>
+        <v>186</v>
       </c>
       <c r="B54" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="B55" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="B56" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>183</v>
+        <v>44</v>
       </c>
       <c r="B57" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B58" t="s">
         <v>159</v>
@@ -1436,207 +1458,207 @@
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B59" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>51</v>
+        <v>179</v>
       </c>
       <c r="B60" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>182</v>
+        <v>47</v>
       </c>
       <c r="B61" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>181</v>
+        <v>48</v>
       </c>
       <c r="B62" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B63" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>53</v>
+        <v>178</v>
       </c>
       <c r="B64" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>54</v>
+        <v>177</v>
       </c>
       <c r="B65" t="s">
-        <v>157</v>
+        <v>162</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="B66" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="B67" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="B68" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="B69" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="B70" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>180</v>
+        <v>55</v>
       </c>
       <c r="B71" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B72" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>191</v>
+        <v>57</v>
       </c>
       <c r="B73" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>189</v>
+        <v>176</v>
       </c>
       <c r="B74" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B75" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>62</v>
+        <v>185</v>
       </c>
       <c r="B76" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>179</v>
+        <v>187</v>
       </c>
       <c r="B77" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B78" t="s">
-        <v>157</v>
+        <v>162</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B79" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="B80" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B81" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>66</v>
+        <v>202</v>
       </c>
       <c r="B82" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="B83" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>68</v>
+        <v>174</v>
       </c>
       <c r="B84" t="s">
         <v>159</v>
@@ -1644,423 +1666,423 @@
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="B85" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="B86" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="B87" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="B88" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="B89" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>177</v>
+        <v>68</v>
       </c>
       <c r="B90" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="B91" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="B92" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="B93" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>77</v>
+        <v>173</v>
       </c>
       <c r="B94" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>176</v>
+        <v>72</v>
       </c>
       <c r="B95" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="B96" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="B97" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="B98" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>81</v>
+        <v>172</v>
       </c>
       <c r="B99" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="B100" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="B101" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="B102" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="B103" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="B104" t="s">
-        <v>157</v>
+        <v>162</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="B105" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="B106" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="B107" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>175</v>
+        <v>83</v>
       </c>
       <c r="B108" t="s">
-        <v>157</v>
+        <v>162</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="B109" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>91</v>
+        <v>194</v>
       </c>
       <c r="B110" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="B111" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="B112" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>174</v>
+        <v>87</v>
       </c>
       <c r="B113" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>94</v>
+        <v>171</v>
       </c>
       <c r="B114" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="B115" t="s">
-        <v>157</v>
+        <v>162</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="B116" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>97</v>
+        <v>195</v>
       </c>
       <c r="B117" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="B118" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>173</v>
+        <v>91</v>
       </c>
       <c r="B119" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>99</v>
+        <v>170</v>
       </c>
       <c r="B120" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>192</v>
+        <v>92</v>
       </c>
       <c r="B121" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="B122" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="B123" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="B124" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="B125" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="B126" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>171</v>
+        <v>97</v>
       </c>
       <c r="B127" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>104</v>
+        <v>188</v>
       </c>
       <c r="B128" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="B129" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>170</v>
+        <v>99</v>
       </c>
       <c r="B130" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="B131" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="B132" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>108</v>
+        <v>168</v>
       </c>
       <c r="B133" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="B134" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="B135" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>111</v>
+        <v>167</v>
       </c>
       <c r="B136" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="B137" t="s">
         <v>158</v>
@@ -2068,151 +2090,151 @@
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>169</v>
+        <v>105</v>
       </c>
       <c r="B138" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="B139" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="B140" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="B141" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="B142" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="B143" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>118</v>
+        <v>166</v>
       </c>
       <c r="B144" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="B145" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="B146" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="B147" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="B148" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="B149" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="B150" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="B151" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="B152" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="B153" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
-        <v>128</v>
+        <v>196</v>
       </c>
       <c r="B154" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="B155" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="B156" t="s">
         <v>159</v>
@@ -2220,175 +2242,175 @@
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="B157" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="B158" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="B159" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="B160" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="B161" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="B162" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
-        <v>137</v>
+        <v>197</v>
       </c>
       <c r="B163" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
-        <v>138</v>
+        <v>128</v>
       </c>
       <c r="B164" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
-        <v>139</v>
+        <v>129</v>
       </c>
       <c r="B165" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
-        <v>140</v>
+        <v>130</v>
       </c>
       <c r="B166" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
-        <v>193</v>
+        <v>131</v>
       </c>
       <c r="B167" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="B168" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="B169" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
-        <v>168</v>
+        <v>134</v>
       </c>
       <c r="B170" t="s">
-        <v>157</v>
+        <v>162</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="B171" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="B172" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="B173" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="B174" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
-        <v>167</v>
+        <v>189</v>
       </c>
       <c r="B175" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="B176" t="s">
-        <v>157</v>
+        <v>162</v>
       </c>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="B177" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
-        <v>149</v>
+        <v>165</v>
       </c>
       <c r="B178" t="s">
         <v>157</v>
@@ -2396,47 +2418,47 @@
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="B179" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="B180" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
-        <v>195</v>
+        <v>143</v>
       </c>
       <c r="B181" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="B182" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
-        <v>153</v>
+        <v>198</v>
       </c>
       <c r="B183" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
-        <v>154</v>
+        <v>164</v>
       </c>
       <c r="B184" t="s">
         <v>158</v>
@@ -2444,26 +2466,98 @@
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
-        <v>155</v>
+        <v>145</v>
       </c>
       <c r="B185" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
-        <v>156</v>
+        <v>146</v>
       </c>
       <c r="B186" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
-        <v>166</v>
+        <v>147</v>
       </c>
       <c r="B187" t="s">
-        <v>161</v>
+        <v>156</v>
+      </c>
+    </row>
+    <row r="188" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A188" t="s">
+        <v>148</v>
+      </c>
+      <c r="B188" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="189" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A189" t="s">
+        <v>149</v>
+      </c>
+      <c r="B189" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="190" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A190" t="s">
+        <v>191</v>
+      </c>
+      <c r="B190" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="191" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A191" t="s">
+        <v>150</v>
+      </c>
+      <c r="B191" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="192" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A192" t="s">
+        <v>151</v>
+      </c>
+      <c r="B192" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="193" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A193" t="s">
+        <v>152</v>
+      </c>
+      <c r="B193" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="194" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A194" t="s">
+        <v>153</v>
+      </c>
+      <c r="B194" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="195" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A195" t="s">
+        <v>154</v>
+      </c>
+      <c r="B195" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="196" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A196" t="s">
+        <v>163</v>
+      </c>
+      <c r="B196" t="s">
+        <v>158</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added column with days since a 100 cases
</commit_message>
<xml_diff>
--- a/region_names.xlsx
+++ b/region_names.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mortenjc/proj/covid2019/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCC31825-42F6-E845-9A58-0F3E185D10DB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0274F3FC-B34B-A04A-B27E-643A1CB1D18F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6880" yWindow="460" windowWidth="16840" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -598,9 +598,6 @@
     <t>United_States_Virgin_Islands</t>
   </si>
   <si>
-    <t>Curaçao</t>
-  </si>
-  <si>
     <t>Laos</t>
   </si>
   <si>
@@ -641,6 +638,9 @@
   </si>
   <si>
     <t>Puerto_Rico</t>
+  </si>
+  <si>
+    <t>Curacao</t>
   </si>
 </sst>
 </file>
@@ -994,8 +994,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B198"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A139" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B150" sqref="B150"/>
+    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A48" sqref="A48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1005,7 +1005,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B1" t="s">
         <v>161</v>
@@ -1069,7 +1069,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B9" t="s">
         <v>159</v>
@@ -1085,7 +1085,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B11" t="s">
         <v>159</v>
@@ -1221,7 +1221,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B28" t="s">
         <v>159</v>
@@ -1381,7 +1381,7 @@
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>192</v>
+        <v>206</v>
       </c>
       <c r="B48" t="s">
         <v>159</v>
@@ -1653,7 +1653,7 @@
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B82" t="s">
         <v>158</v>
@@ -1845,7 +1845,7 @@
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B106" t="s">
         <v>162</v>
@@ -1877,7 +1877,7 @@
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B110" t="s">
         <v>162</v>
@@ -1933,7 +1933,7 @@
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B117" t="s">
         <v>158</v>
@@ -2197,7 +2197,7 @@
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B150" t="s">
         <v>159</v>
@@ -2237,7 +2237,7 @@
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B155" t="s">
         <v>159</v>
@@ -2309,7 +2309,7 @@
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B164" t="s">
         <v>159</v>
@@ -2469,7 +2469,7 @@
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B184" t="s">
         <v>159</v>
@@ -2581,10 +2581,10 @@
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B198" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update with todays numbers
</commit_message>
<xml_diff>
--- a/region_names.xlsx
+++ b/region_names.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mortenjc/proj/covid2019/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7437BA1D-6B7B-454F-88A0-00110E59F0EA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B78647FD-49AE-BC44-82C4-BAF79BBD202F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="12980" yWindow="460" windowWidth="16840" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="217">
   <si>
     <t>Afghanistan</t>
   </si>
@@ -659,6 +659,18 @@
   </si>
   <si>
     <t>South_Sudan</t>
+  </si>
+  <si>
+    <t>Bonaire, Saint Eustatius and Saba</t>
+  </si>
+  <si>
+    <t>Malawi</t>
+  </si>
+  <si>
+    <t>Sao_Tome_and_Principe</t>
+  </si>
+  <si>
+    <t>Yemen</t>
   </si>
 </sst>
 </file>
@@ -1010,10 +1022,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B204"/>
+  <dimension ref="A1:B208"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A153" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A170" sqref="A170"/>
+    <sheetView tabSelected="1" topLeftCell="A189" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A205" sqref="A205"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1223,63 +1235,63 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>19</v>
+        <v>213</v>
       </c>
       <c r="B26" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>207</v>
+        <v>19</v>
       </c>
       <c r="B27" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>20</v>
+        <v>207</v>
       </c>
       <c r="B28" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>200</v>
+        <v>20</v>
       </c>
       <c r="B29" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>21</v>
+        <v>200</v>
       </c>
       <c r="B30" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B31" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B32" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>208</v>
+        <v>23</v>
       </c>
       <c r="B33" t="s">
         <v>158</v>
@@ -1287,63 +1299,63 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>24</v>
+        <v>208</v>
       </c>
       <c r="B34" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B35" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B36" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>182</v>
+        <v>26</v>
       </c>
       <c r="B37" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>27</v>
+        <v>182</v>
       </c>
       <c r="B38" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>181</v>
+        <v>27</v>
       </c>
       <c r="B39" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>28</v>
+        <v>181</v>
       </c>
       <c r="B40" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>180</v>
+        <v>28</v>
       </c>
       <c r="B41" t="s">
         <v>158</v>
@@ -1351,71 +1363,71 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>29</v>
+        <v>180</v>
       </c>
       <c r="B42" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B43" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B44" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B45" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B46" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B47" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B48" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B49" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>206</v>
+        <v>36</v>
       </c>
       <c r="B50" t="s">
         <v>159</v>
@@ -1423,15 +1435,15 @@
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>37</v>
+        <v>206</v>
       </c>
       <c r="B51" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B52" t="s">
         <v>156</v>
@@ -1439,39 +1451,39 @@
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B53" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B54" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B55" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>186</v>
+        <v>41</v>
       </c>
       <c r="B56" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>42</v>
+        <v>186</v>
       </c>
       <c r="B57" t="s">
         <v>159</v>
@@ -1479,39 +1491,39 @@
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B58" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B59" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B60" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B61" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>179</v>
+        <v>46</v>
       </c>
       <c r="B62" t="s">
         <v>158</v>
@@ -1519,23 +1531,23 @@
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>47</v>
+        <v>179</v>
       </c>
       <c r="B63" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B64" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B65" t="s">
         <v>158</v>
@@ -1543,39 +1555,39 @@
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>209</v>
+        <v>49</v>
       </c>
       <c r="B66" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>178</v>
+        <v>209</v>
       </c>
       <c r="B67" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B68" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>50</v>
+        <v>177</v>
       </c>
       <c r="B69" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B70" t="s">
         <v>156</v>
@@ -1583,23 +1595,23 @@
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B71" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B72" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B73" t="s">
         <v>158</v>
@@ -1607,39 +1619,39 @@
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B74" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B75" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B76" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>176</v>
+        <v>57</v>
       </c>
       <c r="B77" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>58</v>
+        <v>176</v>
       </c>
       <c r="B78" t="s">
         <v>156</v>
@@ -1647,55 +1659,55 @@
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>185</v>
+        <v>58</v>
       </c>
       <c r="B79" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B80" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>59</v>
+        <v>187</v>
       </c>
       <c r="B81" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B82" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>175</v>
+        <v>60</v>
       </c>
       <c r="B83" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>61</v>
+        <v>175</v>
       </c>
       <c r="B84" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>201</v>
+        <v>61</v>
       </c>
       <c r="B85" t="s">
         <v>158</v>
@@ -1703,47 +1715,47 @@
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>62</v>
+        <v>201</v>
       </c>
       <c r="B86" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>174</v>
+        <v>62</v>
       </c>
       <c r="B87" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>63</v>
+        <v>174</v>
       </c>
       <c r="B88" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B89" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B90" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B91" t="s">
         <v>156</v>
@@ -1751,15 +1763,15 @@
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B92" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B93" t="s">
         <v>162</v>
@@ -1767,7 +1779,7 @@
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B94" t="s">
         <v>162</v>
@@ -1775,7 +1787,7 @@
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B95" t="s">
         <v>162</v>
@@ -1783,15 +1795,15 @@
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B96" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>173</v>
+        <v>71</v>
       </c>
       <c r="B97" t="s">
         <v>156</v>
@@ -1799,55 +1811,55 @@
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>72</v>
+        <v>173</v>
       </c>
       <c r="B98" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B99" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B100" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B101" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>172</v>
+        <v>75</v>
       </c>
       <c r="B102" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>76</v>
+        <v>172</v>
       </c>
       <c r="B103" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B104" t="s">
         <v>162</v>
@@ -1855,31 +1867,31 @@
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B105" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B106" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B107" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B108" t="s">
         <v>162</v>
@@ -1887,7 +1899,7 @@
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>192</v>
+        <v>81</v>
       </c>
       <c r="B109" t="s">
         <v>162</v>
@@ -1895,47 +1907,47 @@
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>82</v>
+        <v>192</v>
       </c>
       <c r="B110" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B111" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B112" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>193</v>
+        <v>84</v>
       </c>
       <c r="B113" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>85</v>
+        <v>193</v>
       </c>
       <c r="B114" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B115" t="s">
         <v>156</v>
@@ -1943,7 +1955,7 @@
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B116" t="s">
         <v>156</v>
@@ -1951,47 +1963,47 @@
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>171</v>
+        <v>87</v>
       </c>
       <c r="B117" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>88</v>
+        <v>171</v>
       </c>
       <c r="B118" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>89</v>
+        <v>214</v>
       </c>
       <c r="B119" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>194</v>
+        <v>88</v>
       </c>
       <c r="B120" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B121" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>91</v>
+        <v>194</v>
       </c>
       <c r="B122" t="s">
         <v>158</v>
@@ -1999,47 +2011,47 @@
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>170</v>
+        <v>90</v>
       </c>
       <c r="B123" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B124" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>93</v>
+        <v>170</v>
       </c>
       <c r="B125" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B126" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B127" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B128" t="s">
         <v>156</v>
@@ -2047,39 +2059,39 @@
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>169</v>
+        <v>95</v>
       </c>
       <c r="B129" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B130" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>188</v>
+        <v>169</v>
       </c>
       <c r="B131" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B132" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>99</v>
+        <v>188</v>
       </c>
       <c r="B133" t="s">
         <v>158</v>
@@ -2087,7 +2099,7 @@
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B134" t="s">
         <v>162</v>
@@ -2095,71 +2107,71 @@
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B135" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>168</v>
+        <v>100</v>
       </c>
       <c r="B136" t="s">
-        <v>157</v>
+        <v>162</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B137" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>103</v>
+        <v>168</v>
       </c>
       <c r="B138" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>167</v>
+        <v>102</v>
       </c>
       <c r="B139" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B140" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>105</v>
+        <v>167</v>
       </c>
       <c r="B141" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>210</v>
+        <v>104</v>
       </c>
       <c r="B142" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B143" t="s">
         <v>156</v>
@@ -2167,47 +2179,47 @@
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>107</v>
+        <v>210</v>
       </c>
       <c r="B144" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B145" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B146" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B147" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>166</v>
+        <v>109</v>
       </c>
       <c r="B148" t="s">
-        <v>157</v>
+        <v>162</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B149" t="s">
         <v>155</v>
@@ -2215,95 +2227,95 @@
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>112</v>
+        <v>166</v>
       </c>
       <c r="B150" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B151" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B152" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B153" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
-        <v>205</v>
+        <v>114</v>
       </c>
       <c r="B154" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B155" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
-        <v>117</v>
+        <v>205</v>
       </c>
       <c r="B156" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B157" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B158" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
-        <v>195</v>
+        <v>118</v>
       </c>
       <c r="B159" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B160" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
-        <v>121</v>
+        <v>195</v>
       </c>
       <c r="B161" t="s">
         <v>159</v>
@@ -2311,47 +2323,47 @@
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B162" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B163" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B164" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
-        <v>125</v>
+        <v>215</v>
       </c>
       <c r="B165" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B166" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
-        <v>211</v>
+        <v>124</v>
       </c>
       <c r="B167" t="s">
         <v>158</v>
@@ -2359,63 +2371,63 @@
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B168" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
-        <v>196</v>
+        <v>126</v>
       </c>
       <c r="B169" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
-        <v>128</v>
+        <v>211</v>
       </c>
       <c r="B170" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B171" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
-        <v>130</v>
+        <v>196</v>
       </c>
       <c r="B172" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B173" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B174" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
-        <v>212</v>
+        <v>130</v>
       </c>
       <c r="B175" t="s">
         <v>158</v>
@@ -2423,15 +2435,15 @@
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B176" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B177" t="s">
         <v>162</v>
@@ -2439,7 +2451,7 @@
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
-        <v>135</v>
+        <v>212</v>
       </c>
       <c r="B178" t="s">
         <v>158</v>
@@ -2447,103 +2459,103 @@
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="B179" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B180" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="B181" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
-        <v>189</v>
+        <v>136</v>
       </c>
       <c r="B182" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B183" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B184" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
-        <v>165</v>
+        <v>189</v>
       </c>
       <c r="B185" t="s">
-        <v>157</v>
+        <v>162</v>
       </c>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B186" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B187" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
-        <v>143</v>
+        <v>165</v>
       </c>
       <c r="B188" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="B189" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
-        <v>197</v>
+        <v>142</v>
       </c>
       <c r="B190" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
-        <v>164</v>
+        <v>143</v>
       </c>
       <c r="B191" t="s">
         <v>158</v>
@@ -2551,7 +2563,7 @@
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B192" t="s">
         <v>156</v>
@@ -2559,97 +2571,129 @@
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
-        <v>146</v>
+        <v>197</v>
       </c>
       <c r="B193" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
-        <v>147</v>
+        <v>164</v>
       </c>
       <c r="B194" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="B195" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="B196" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
-        <v>191</v>
+        <v>147</v>
       </c>
       <c r="B197" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B198" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B199" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
-        <v>152</v>
+        <v>191</v>
       </c>
       <c r="B200" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="B201" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="B202" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
-        <v>163</v>
+        <v>152</v>
       </c>
       <c r="B203" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
+        <v>153</v>
+      </c>
+      <c r="B204" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="205" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A205" t="s">
+        <v>216</v>
+      </c>
+      <c r="B205" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="206" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A206" t="s">
+        <v>154</v>
+      </c>
+      <c r="B206" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="207" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A207" t="s">
+        <v>163</v>
+      </c>
+      <c r="B207" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="208" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A208" t="s">
         <v>204</v>
       </c>
-      <c r="B204" t="s">
+      <c r="B208" t="s">
         <v>203</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update with latest cases
</commit_message>
<xml_diff>
--- a/region_names.xlsx
+++ b/region_names.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mortenjc/proj/covid2019/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B78647FD-49AE-BC44-82C4-BAF79BBD202F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A83BF930-1A0F-384D-82A5-4CDC9EB52025}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12980" yWindow="460" windowWidth="16840" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10460" yWindow="460" windowWidth="16840" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="countries" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="218">
   <si>
     <t>Afghanistan</t>
   </si>
@@ -136,9 +136,6 @@
     <t>Cyprus</t>
   </si>
   <si>
-    <t>Czech_Republic</t>
-  </si>
-  <si>
     <t>Democratic_Republic_of_the_Congo</t>
   </si>
   <si>
@@ -640,9 +637,6 @@
     <t>Puerto_Rico</t>
   </si>
   <si>
-    <t>Curaçao</t>
-  </si>
-  <si>
     <t>Botswana</t>
   </si>
   <si>
@@ -671,6 +665,15 @@
   </si>
   <si>
     <t>Yemen</t>
+  </si>
+  <si>
+    <t>CuraÃ§ao</t>
+  </si>
+  <si>
+    <t>Czechia</t>
+  </si>
+  <si>
+    <t>Western_Sahara</t>
   </si>
 </sst>
 </file>
@@ -1022,10 +1025,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B208"/>
+  <dimension ref="A1:B209"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A189" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A205" sqref="A205"/>
+    <sheetView tabSelected="1" topLeftCell="A179" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A201" sqref="A201"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1035,10 +1038,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -1046,15 +1049,15 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -1062,7 +1065,7 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -1070,7 +1073,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -1078,7 +1081,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -1086,7 +1089,7 @@
         <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
@@ -1094,15 +1097,15 @@
         <v>2</v>
       </c>
       <c r="B8" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B9" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
@@ -1110,15 +1113,15 @@
         <v>6</v>
       </c>
       <c r="B10" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B11" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
@@ -1126,7 +1129,7 @@
         <v>7</v>
       </c>
       <c r="B12" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
@@ -1134,7 +1137,7 @@
         <v>8</v>
       </c>
       <c r="B13" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
@@ -1142,7 +1145,7 @@
         <v>9</v>
       </c>
       <c r="B14" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
@@ -1150,7 +1153,7 @@
         <v>10</v>
       </c>
       <c r="B15" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
@@ -1158,7 +1161,7 @@
         <v>11</v>
       </c>
       <c r="B16" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
@@ -1166,7 +1169,7 @@
         <v>12</v>
       </c>
       <c r="B17" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
@@ -1174,7 +1177,7 @@
         <v>13</v>
       </c>
       <c r="B18" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
@@ -1182,7 +1185,7 @@
         <v>14</v>
       </c>
       <c r="B19" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
@@ -1190,15 +1193,15 @@
         <v>15</v>
       </c>
       <c r="B20" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B21" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
@@ -1206,15 +1209,15 @@
         <v>16</v>
       </c>
       <c r="B22" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B23" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
@@ -1222,7 +1225,7 @@
         <v>17</v>
       </c>
       <c r="B24" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
@@ -1230,15 +1233,15 @@
         <v>18</v>
       </c>
       <c r="B25" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B26" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
@@ -1246,15 +1249,15 @@
         <v>19</v>
       </c>
       <c r="B27" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B28" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
@@ -1262,15 +1265,15 @@
         <v>20</v>
       </c>
       <c r="B29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B30" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
@@ -1278,7 +1281,7 @@
         <v>21</v>
       </c>
       <c r="B31" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
@@ -1286,7 +1289,7 @@
         <v>22</v>
       </c>
       <c r="B32" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
@@ -1294,15 +1297,15 @@
         <v>23</v>
       </c>
       <c r="B33" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B34" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
@@ -1310,7 +1313,7 @@
         <v>24</v>
       </c>
       <c r="B35" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
@@ -1318,7 +1321,7 @@
         <v>25</v>
       </c>
       <c r="B36" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
@@ -1326,15 +1329,15 @@
         <v>26</v>
       </c>
       <c r="B37" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B38" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
@@ -1342,15 +1345,15 @@
         <v>27</v>
       </c>
       <c r="B39" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B40" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
@@ -1358,15 +1361,15 @@
         <v>28</v>
       </c>
       <c r="B41" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B42" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
@@ -1374,7 +1377,7 @@
         <v>29</v>
       </c>
       <c r="B43" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
@@ -1382,7 +1385,7 @@
         <v>30</v>
       </c>
       <c r="B44" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
@@ -1390,7 +1393,7 @@
         <v>31</v>
       </c>
       <c r="B45" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
@@ -1398,7 +1401,7 @@
         <v>32</v>
       </c>
       <c r="B46" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
@@ -1406,7 +1409,7 @@
         <v>33</v>
       </c>
       <c r="B47" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
@@ -1414,7 +1417,7 @@
         <v>34</v>
       </c>
       <c r="B48" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
@@ -1422,7 +1425,7 @@
         <v>35</v>
       </c>
       <c r="B49" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
@@ -1430,15 +1433,15 @@
         <v>36</v>
       </c>
       <c r="B50" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>206</v>
+        <v>215</v>
       </c>
       <c r="B51" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
@@ -1446,1255 +1449,1263 @@
         <v>37</v>
       </c>
       <c r="B52" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>38</v>
+        <v>216</v>
       </c>
       <c r="B53" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B54" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B55" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B56" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B57" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B58" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B59" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B60" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B61" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B62" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B63" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B64" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B65" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B66" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B67" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B68" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B69" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B70" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B71" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B72" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B73" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B74" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B75" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B76" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B77" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B78" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B79" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B80" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B81" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B82" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B83" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B84" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B85" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B86" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B87" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B88" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B89" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B90" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B91" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B92" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B93" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B94" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B95" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B96" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B97" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B98" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B99" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B100" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B101" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B102" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B103" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B104" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B105" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B106" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B107" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B108" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B109" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B110" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B111" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B112" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B113" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B114" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B115" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B116" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B117" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B118" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B119" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B120" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B121" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B122" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B123" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B124" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B125" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B126" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B127" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B128" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B129" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B130" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B131" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B132" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B133" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B134" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B135" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B136" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B137" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B138" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B139" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B140" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B141" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B142" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B143" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B144" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B145" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B146" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B147" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B148" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B149" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B150" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B151" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B152" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B153" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B154" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B155" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B156" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B157" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B158" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B159" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B160" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B161" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B162" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B163" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B164" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B165" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B166" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B167" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B168" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B169" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B170" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B171" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B172" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B173" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B174" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B175" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B176" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B177" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B178" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B179" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B180" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B181" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B182" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B183" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B184" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B185" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B186" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B187" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B188" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B189" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B190" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B191" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B192" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B193" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B194" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B195" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B196" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B197" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B198" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B199" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B200" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B201" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B202" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B203" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B204" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="205" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="B205" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
     </row>
     <row r="206" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
-        <v>154</v>
+        <v>214</v>
       </c>
       <c r="B206" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
     </row>
     <row r="207" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
-        <v>163</v>
+        <v>153</v>
       </c>
       <c r="B207" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="208" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
-        <v>204</v>
+        <v>162</v>
       </c>
       <c r="B208" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="209" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A209" t="s">
         <v>203</v>
+      </c>
+      <c r="B209" t="s">
+        <v>202</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update w. latest data
</commit_message>
<xml_diff>
--- a/region_names.xlsx
+++ b/region_names.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mortenjc/proj/covid2019/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A83BF930-1A0F-384D-82A5-4CDC9EB52025}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F819166B-021D-BE4C-8DF4-A1399E581158}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10460" yWindow="460" windowWidth="16840" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="220">
   <si>
     <t>Afghanistan</t>
   </si>
@@ -674,6 +674,12 @@
   </si>
   <si>
     <t>Western_Sahara</t>
+  </si>
+  <si>
+    <t>Comoros</t>
+  </si>
+  <si>
+    <t>Tajikistan</t>
   </si>
 </sst>
 </file>
@@ -1025,10 +1031,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B209"/>
+  <dimension ref="A1:B211"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A179" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A201" sqref="A201"/>
+    <sheetView tabSelected="1" topLeftCell="A170" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B189" sqref="B189"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1398,7 +1404,7 @@
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>32</v>
+        <v>218</v>
       </c>
       <c r="B46" t="s">
         <v>157</v>
@@ -1406,39 +1412,39 @@
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B47" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B48" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B49" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B50" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>215</v>
+        <v>36</v>
       </c>
       <c r="B51" t="s">
         <v>158</v>
@@ -1446,15 +1452,15 @@
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>37</v>
+        <v>215</v>
       </c>
       <c r="B52" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>216</v>
+        <v>37</v>
       </c>
       <c r="B53" t="s">
         <v>155</v>
@@ -1462,39 +1468,39 @@
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>38</v>
+        <v>216</v>
       </c>
       <c r="B54" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B55" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B56" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>185</v>
+        <v>40</v>
       </c>
       <c r="B57" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>41</v>
+        <v>185</v>
       </c>
       <c r="B58" t="s">
         <v>158</v>
@@ -1502,39 +1508,39 @@
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B59" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B60" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B61" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B62" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>178</v>
+        <v>45</v>
       </c>
       <c r="B63" t="s">
         <v>157</v>
@@ -1542,23 +1548,23 @@
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>46</v>
+        <v>178</v>
       </c>
       <c r="B64" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B65" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B66" t="s">
         <v>157</v>
@@ -1566,39 +1572,39 @@
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>207</v>
+        <v>48</v>
       </c>
       <c r="B67" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>177</v>
+        <v>207</v>
       </c>
       <c r="B68" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B69" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>49</v>
+        <v>176</v>
       </c>
       <c r="B70" t="s">
-        <v>155</v>
+        <v>161</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B71" t="s">
         <v>155</v>
@@ -1606,23 +1612,23 @@
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B72" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B73" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B74" t="s">
         <v>157</v>
@@ -1630,39 +1636,39 @@
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B75" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B76" t="s">
-        <v>155</v>
+        <v>161</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B77" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>175</v>
+        <v>56</v>
       </c>
       <c r="B78" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>57</v>
+        <v>175</v>
       </c>
       <c r="B79" t="s">
         <v>155</v>
@@ -1670,55 +1676,55 @@
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>184</v>
+        <v>57</v>
       </c>
       <c r="B80" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B81" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>58</v>
+        <v>186</v>
       </c>
       <c r="B82" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B83" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>174</v>
+        <v>59</v>
       </c>
       <c r="B84" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>60</v>
+        <v>174</v>
       </c>
       <c r="B85" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>200</v>
+        <v>60</v>
       </c>
       <c r="B86" t="s">
         <v>157</v>
@@ -1726,47 +1732,47 @@
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>61</v>
+        <v>200</v>
       </c>
       <c r="B87" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>173</v>
+        <v>61</v>
       </c>
       <c r="B88" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>62</v>
+        <v>173</v>
       </c>
       <c r="B89" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B90" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B91" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B92" t="s">
         <v>155</v>
@@ -1774,15 +1780,15 @@
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B93" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B94" t="s">
         <v>161</v>
@@ -1790,7 +1796,7 @@
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B95" t="s">
         <v>161</v>
@@ -1798,7 +1804,7 @@
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B96" t="s">
         <v>161</v>
@@ -1806,15 +1812,15 @@
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B97" t="s">
-        <v>155</v>
+        <v>161</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>172</v>
+        <v>70</v>
       </c>
       <c r="B98" t="s">
         <v>155</v>
@@ -1822,55 +1828,55 @@
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>71</v>
+        <v>172</v>
       </c>
       <c r="B99" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B100" t="s">
-        <v>155</v>
+        <v>161</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B101" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B102" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>171</v>
+        <v>74</v>
       </c>
       <c r="B103" t="s">
-        <v>155</v>
+        <v>161</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>75</v>
+        <v>171</v>
       </c>
       <c r="B104" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B105" t="s">
         <v>161</v>
@@ -1878,31 +1884,31 @@
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B106" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B107" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B108" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B109" t="s">
         <v>161</v>
@@ -1910,7 +1916,7 @@
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>191</v>
+        <v>80</v>
       </c>
       <c r="B110" t="s">
         <v>161</v>
@@ -1918,47 +1924,47 @@
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>81</v>
+        <v>191</v>
       </c>
       <c r="B111" t="s">
-        <v>155</v>
+        <v>161</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B112" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B113" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>192</v>
+        <v>83</v>
       </c>
       <c r="B114" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>84</v>
+        <v>192</v>
       </c>
       <c r="B115" t="s">
-        <v>155</v>
+        <v>161</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B116" t="s">
         <v>155</v>
@@ -1966,7 +1972,7 @@
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B117" t="s">
         <v>155</v>
@@ -1974,15 +1980,15 @@
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>170</v>
+        <v>86</v>
       </c>
       <c r="B118" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>212</v>
+        <v>170</v>
       </c>
       <c r="B119" t="s">
         <v>157</v>
@@ -1990,15 +1996,15 @@
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>87</v>
+        <v>212</v>
       </c>
       <c r="B120" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B121" t="s">
         <v>161</v>
@@ -2006,31 +2012,31 @@
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>193</v>
+        <v>88</v>
       </c>
       <c r="B122" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>89</v>
+        <v>193</v>
       </c>
       <c r="B123" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B124" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>169</v>
+        <v>90</v>
       </c>
       <c r="B125" t="s">
         <v>157</v>
@@ -2038,23 +2044,23 @@
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>91</v>
+        <v>169</v>
       </c>
       <c r="B126" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B127" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B128" t="s">
         <v>155</v>
@@ -2062,23 +2068,23 @@
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B129" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B130" t="s">
-        <v>155</v>
+        <v>161</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>168</v>
+        <v>95</v>
       </c>
       <c r="B131" t="s">
         <v>155</v>
@@ -2086,15 +2092,15 @@
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>96</v>
+        <v>168</v>
       </c>
       <c r="B132" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>187</v>
+        <v>96</v>
       </c>
       <c r="B133" t="s">
         <v>157</v>
@@ -2102,47 +2108,47 @@
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>97</v>
+        <v>187</v>
       </c>
       <c r="B134" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B135" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B136" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B137" t="s">
-        <v>155</v>
+        <v>161</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>167</v>
+        <v>100</v>
       </c>
       <c r="B138" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>101</v>
+        <v>167</v>
       </c>
       <c r="B139" t="s">
         <v>156</v>
@@ -2150,23 +2156,23 @@
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B140" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>166</v>
+        <v>102</v>
       </c>
       <c r="B141" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>103</v>
+        <v>166</v>
       </c>
       <c r="B142" t="s">
         <v>157</v>
@@ -2174,47 +2180,47 @@
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B143" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>208</v>
+        <v>104</v>
       </c>
       <c r="B144" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>105</v>
+        <v>208</v>
       </c>
       <c r="B145" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B146" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B147" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B148" t="s">
         <v>161</v>
@@ -2222,31 +2228,31 @@
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B149" t="s">
-        <v>154</v>
+        <v>161</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>165</v>
+        <v>109</v>
       </c>
       <c r="B150" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>110</v>
+        <v>165</v>
       </c>
       <c r="B151" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B152" t="s">
         <v>154</v>
@@ -2254,23 +2260,23 @@
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B153" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B154" t="s">
-        <v>155</v>
+        <v>161</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B155" t="s">
         <v>155</v>
@@ -2278,31 +2284,31 @@
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
-        <v>204</v>
+        <v>114</v>
       </c>
       <c r="B156" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
-        <v>115</v>
+        <v>204</v>
       </c>
       <c r="B157" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B158" t="s">
-        <v>155</v>
+        <v>161</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B159" t="s">
         <v>155</v>
@@ -2310,23 +2316,23 @@
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B160" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
-        <v>194</v>
+        <v>118</v>
       </c>
       <c r="B161" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
-        <v>119</v>
+        <v>194</v>
       </c>
       <c r="B162" t="s">
         <v>158</v>
@@ -2334,7 +2340,7 @@
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B163" t="s">
         <v>158</v>
@@ -2342,55 +2348,55 @@
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B164" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
-        <v>213</v>
+        <v>121</v>
       </c>
       <c r="B165" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
-        <v>122</v>
+        <v>213</v>
       </c>
       <c r="B166" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B167" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B168" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B169" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
-        <v>209</v>
+        <v>125</v>
       </c>
       <c r="B170" t="s">
         <v>157</v>
@@ -2398,31 +2404,31 @@
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
-        <v>126</v>
+        <v>209</v>
       </c>
       <c r="B171" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
-        <v>195</v>
+        <v>126</v>
       </c>
       <c r="B172" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
-        <v>127</v>
+        <v>195</v>
       </c>
       <c r="B173" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B174" t="s">
         <v>155</v>
@@ -2430,15 +2436,15 @@
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B175" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B176" t="s">
         <v>157</v>
@@ -2446,63 +2452,63 @@
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B177" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
-        <v>210</v>
+        <v>131</v>
       </c>
       <c r="B178" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
-        <v>132</v>
+        <v>210</v>
       </c>
       <c r="B179" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B180" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B181" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B182" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B183" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B184" t="s">
         <v>155</v>
@@ -2510,15 +2516,15 @@
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
-        <v>188</v>
+        <v>137</v>
       </c>
       <c r="B185" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
-        <v>138</v>
+        <v>188</v>
       </c>
       <c r="B186" t="s">
         <v>161</v>
@@ -2526,7 +2532,7 @@
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B187" t="s">
         <v>161</v>
@@ -2534,31 +2540,31 @@
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
-        <v>164</v>
+        <v>219</v>
       </c>
       <c r="B188" t="s">
-        <v>156</v>
+        <v>161</v>
       </c>
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B189" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
-        <v>141</v>
+        <v>164</v>
       </c>
       <c r="B190" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B191" t="s">
         <v>157</v>
@@ -2566,47 +2572,47 @@
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B192" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
-        <v>196</v>
+        <v>142</v>
       </c>
       <c r="B193" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
-        <v>163</v>
+        <v>143</v>
       </c>
       <c r="B194" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
-        <v>144</v>
+        <v>196</v>
       </c>
       <c r="B195" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
-        <v>145</v>
+        <v>163</v>
       </c>
       <c r="B196" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B197" t="s">
         <v>155</v>
@@ -2614,47 +2620,47 @@
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B198" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B199" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
-        <v>190</v>
+        <v>147</v>
       </c>
       <c r="B200" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B201" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
-        <v>150</v>
+        <v>190</v>
       </c>
       <c r="B202" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B203" t="s">
         <v>154</v>
@@ -2662,7 +2668,7 @@
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B204" t="s">
         <v>161</v>
@@ -2670,15 +2676,15 @@
     </row>
     <row r="205" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
-        <v>217</v>
+        <v>151</v>
       </c>
       <c r="B205" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="206" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
-        <v>214</v>
+        <v>152</v>
       </c>
       <c r="B206" t="s">
         <v>161</v>
@@ -2686,7 +2692,7 @@
     </row>
     <row r="207" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
-        <v>153</v>
+        <v>217</v>
       </c>
       <c r="B207" t="s">
         <v>157</v>
@@ -2694,17 +2700,33 @@
     </row>
     <row r="208" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
-        <v>162</v>
+        <v>214</v>
       </c>
       <c r="B208" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
     </row>
     <row r="209" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
+        <v>153</v>
+      </c>
+      <c r="B209" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="210" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A210" t="s">
+        <v>162</v>
+      </c>
+      <c r="B210" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="211" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A211" t="s">
         <v>203</v>
       </c>
-      <c r="B209" t="s">
+      <c r="B211" t="s">
         <v>202</v>
       </c>
     </row>

</xml_diff>

<commit_message>
faster reads from excel, added assert, refactor
</commit_message>
<xml_diff>
--- a/region_names.xlsx
+++ b/region_names.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mortenjc/proj/covid2019/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F819166B-021D-BE4C-8DF4-A1399E581158}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8F53E96-5F78-2E43-840D-9CE2BB51106D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10460" yWindow="460" windowWidth="16840" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="221">
   <si>
     <t>Afghanistan</t>
   </si>
@@ -680,6 +680,9 @@
   </si>
   <si>
     <t>Tajikistan</t>
+  </si>
+  <si>
+    <t>Lesotho</t>
   </si>
 </sst>
 </file>
@@ -1031,10 +1034,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B211"/>
+  <dimension ref="A1:B212"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A170" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B189" sqref="B189"/>
+    <sheetView tabSelected="1" topLeftCell="A98" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A114" sqref="A114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1948,7 +1951,7 @@
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>83</v>
+        <v>220</v>
       </c>
       <c r="B114" t="s">
         <v>157</v>
@@ -1956,23 +1959,23 @@
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>192</v>
+        <v>83</v>
       </c>
       <c r="B115" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>84</v>
+        <v>192</v>
       </c>
       <c r="B116" t="s">
-        <v>155</v>
+        <v>161</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B117" t="s">
         <v>155</v>
@@ -1980,7 +1983,7 @@
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B118" t="s">
         <v>155</v>
@@ -1988,15 +1991,15 @@
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>170</v>
+        <v>86</v>
       </c>
       <c r="B119" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>212</v>
+        <v>170</v>
       </c>
       <c r="B120" t="s">
         <v>157</v>
@@ -2004,15 +2007,15 @@
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>87</v>
+        <v>212</v>
       </c>
       <c r="B121" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B122" t="s">
         <v>161</v>
@@ -2020,31 +2023,31 @@
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>193</v>
+        <v>88</v>
       </c>
       <c r="B123" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>89</v>
+        <v>193</v>
       </c>
       <c r="B124" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B125" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>169</v>
+        <v>90</v>
       </c>
       <c r="B126" t="s">
         <v>157</v>
@@ -2052,23 +2055,23 @@
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>91</v>
+        <v>169</v>
       </c>
       <c r="B127" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B128" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B129" t="s">
         <v>155</v>
@@ -2076,23 +2079,23 @@
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B130" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B131" t="s">
-        <v>155</v>
+        <v>161</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>168</v>
+        <v>95</v>
       </c>
       <c r="B132" t="s">
         <v>155</v>
@@ -2100,15 +2103,15 @@
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>96</v>
+        <v>168</v>
       </c>
       <c r="B133" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>187</v>
+        <v>96</v>
       </c>
       <c r="B134" t="s">
         <v>157</v>
@@ -2116,47 +2119,47 @@
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>97</v>
+        <v>187</v>
       </c>
       <c r="B135" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B136" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B137" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B138" t="s">
-        <v>155</v>
+        <v>161</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>167</v>
+        <v>100</v>
       </c>
       <c r="B139" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>101</v>
+        <v>167</v>
       </c>
       <c r="B140" t="s">
         <v>156</v>
@@ -2164,23 +2167,23 @@
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B141" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>166</v>
+        <v>102</v>
       </c>
       <c r="B142" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>103</v>
+        <v>166</v>
       </c>
       <c r="B143" t="s">
         <v>157</v>
@@ -2188,47 +2191,47 @@
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B144" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>208</v>
+        <v>104</v>
       </c>
       <c r="B145" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>105</v>
+        <v>208</v>
       </c>
       <c r="B146" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B147" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B148" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B149" t="s">
         <v>161</v>
@@ -2236,31 +2239,31 @@
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B150" t="s">
-        <v>154</v>
+        <v>161</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>165</v>
+        <v>109</v>
       </c>
       <c r="B151" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
-        <v>110</v>
+        <v>165</v>
       </c>
       <c r="B152" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B153" t="s">
         <v>154</v>
@@ -2268,23 +2271,23 @@
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B154" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B155" t="s">
-        <v>155</v>
+        <v>161</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B156" t="s">
         <v>155</v>
@@ -2292,31 +2295,31 @@
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
-        <v>204</v>
+        <v>114</v>
       </c>
       <c r="B157" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
-        <v>115</v>
+        <v>204</v>
       </c>
       <c r="B158" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B159" t="s">
-        <v>155</v>
+        <v>161</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B160" t="s">
         <v>155</v>
@@ -2324,23 +2327,23 @@
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B161" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
-        <v>194</v>
+        <v>118</v>
       </c>
       <c r="B162" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
-        <v>119</v>
+        <v>194</v>
       </c>
       <c r="B163" t="s">
         <v>158</v>
@@ -2348,7 +2351,7 @@
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B164" t="s">
         <v>158</v>
@@ -2356,55 +2359,55 @@
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B165" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
-        <v>213</v>
+        <v>121</v>
       </c>
       <c r="B166" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
-        <v>122</v>
+        <v>213</v>
       </c>
       <c r="B167" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B168" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B169" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B170" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
-        <v>209</v>
+        <v>125</v>
       </c>
       <c r="B171" t="s">
         <v>157</v>
@@ -2412,31 +2415,31 @@
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
-        <v>126</v>
+        <v>209</v>
       </c>
       <c r="B172" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
-        <v>195</v>
+        <v>126</v>
       </c>
       <c r="B173" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
-        <v>127</v>
+        <v>195</v>
       </c>
       <c r="B174" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B175" t="s">
         <v>155</v>
@@ -2444,15 +2447,15 @@
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B176" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B177" t="s">
         <v>157</v>
@@ -2460,63 +2463,63 @@
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B178" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
-        <v>210</v>
+        <v>131</v>
       </c>
       <c r="B179" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
-        <v>132</v>
+        <v>210</v>
       </c>
       <c r="B180" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B181" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B182" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B183" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B184" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B185" t="s">
         <v>155</v>
@@ -2524,15 +2527,15 @@
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
-        <v>188</v>
+        <v>137</v>
       </c>
       <c r="B186" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
-        <v>138</v>
+        <v>188</v>
       </c>
       <c r="B187" t="s">
         <v>161</v>
@@ -2540,7 +2543,7 @@
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
-        <v>219</v>
+        <v>138</v>
       </c>
       <c r="B188" t="s">
         <v>161</v>
@@ -2548,7 +2551,7 @@
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
-        <v>139</v>
+        <v>219</v>
       </c>
       <c r="B189" t="s">
         <v>161</v>
@@ -2556,103 +2559,103 @@
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
-        <v>164</v>
+        <v>139</v>
       </c>
       <c r="B190" t="s">
-        <v>156</v>
+        <v>161</v>
       </c>
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
-        <v>140</v>
+        <v>164</v>
       </c>
       <c r="B191" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B192" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B193" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B194" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
-        <v>196</v>
+        <v>143</v>
       </c>
       <c r="B195" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
-        <v>163</v>
+        <v>196</v>
       </c>
       <c r="B196" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
-        <v>144</v>
+        <v>163</v>
       </c>
       <c r="B197" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B198" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B199" t="s">
-        <v>155</v>
+        <v>161</v>
       </c>
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B200" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B201" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
-        <v>190</v>
+        <v>148</v>
       </c>
       <c r="B202" t="s">
         <v>158</v>
@@ -2660,63 +2663,63 @@
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
-        <v>149</v>
+        <v>190</v>
       </c>
       <c r="B203" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B204" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
     </row>
     <row r="205" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B205" t="s">
-        <v>154</v>
+        <v>161</v>
       </c>
     </row>
     <row r="206" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B206" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
     </row>
     <row r="207" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
-        <v>217</v>
+        <v>152</v>
       </c>
       <c r="B207" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
     </row>
     <row r="208" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="B208" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
     </row>
     <row r="209" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
-        <v>153</v>
+        <v>214</v>
       </c>
       <c r="B209" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
     </row>
     <row r="210" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A210" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
       <c r="B210" t="s">
         <v>157</v>
@@ -2724,9 +2727,17 @@
     </row>
     <row r="211" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A211" t="s">
+        <v>162</v>
+      </c>
+      <c r="B211" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="212" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A212" t="s">
         <v>203</v>
       </c>
-      <c r="B211" t="s">
+      <c r="B212" t="s">
         <v>202</v>
       </c>
     </row>

</xml_diff>